<commit_message>
Corrigindo erro no excell
</commit_message>
<xml_diff>
--- a/podcastapp/analiseViaExcell/Análise de requisitos.xlsx
+++ b/podcastapp/analiseViaExcell/Análise de requisitos.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jegef\Desktop\Metodo PDA\portifolio-analise\podcastapp\analiseViaExcell\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23F4E01E-9716-4171-B7A5-77F336FCCBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19455" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Numero</t>
   </si>
@@ -57,13 +66,6 @@
   </si>
   <si>
     <t>Categorias Podcast</t>
-  </si>
-  <si>
-    <t>regra de negócio 1
-regra de negócio 2
-regra de negócio 3
-regra de negócio 4
-regra de negócio 5</t>
   </si>
   <si>
     <t>Podcast Recomendados</t>
@@ -122,15 +124,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -141,53 +144,76 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="85725" cy="200025"/>
+    <xdr:ext cx="704850" cy="790575"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="2" name="image1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5591175" y="247650"/>
+          <a:ext cx="704850" cy="790575"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -199,23 +225,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="104775" cy="200025"/>
+    <xdr:ext cx="371475" cy="523875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png"/>
+        <xdr:cNvPr id="3" name="image7.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="1181100"/>
+          <a:ext cx="371475" cy="523875"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -227,23 +263,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="95250" cy="200025"/>
+    <xdr:ext cx="495300" cy="771525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png"/>
+        <xdr:cNvPr id="4" name="image5.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5676900" y="1857375"/>
+          <a:ext cx="495300" cy="771525"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -255,23 +301,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="95250" cy="200025"/>
+    <xdr:ext cx="571500" cy="666750"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png"/>
+        <xdr:cNvPr id="5" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5667375" y="2876550"/>
+          <a:ext cx="571500" cy="666750"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -283,23 +339,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="95250" cy="200025"/>
+    <xdr:ext cx="323850" cy="819150"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="6" name="image2.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5753100" y="3790950"/>
+          <a:ext cx="323850" cy="819150"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -311,23 +377,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="66675" cy="200025"/>
+    <xdr:ext cx="695325" cy="1457325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png"/>
+        <xdr:cNvPr id="7" name="image3.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5638800" y="4895850"/>
+          <a:ext cx="695325" cy="1457325"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -339,23 +415,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="57150" cy="200025"/>
+    <xdr:ext cx="495300" cy="1676400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png"/>
+        <xdr:cNvPr id="8" name="image8.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5734050" y="7162800"/>
+          <a:ext cx="495300" cy="1676400"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -367,23 +453,33 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="76200" cy="200025"/>
+    <xdr:ext cx="552450" cy="1190625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png"/>
+        <xdr:cNvPr id="9" name="image6.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5676900" y="9582150"/>
+          <a:ext cx="552450" cy="1190625"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -396,7 +492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -586,24 +682,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="19.63"/>
-    <col customWidth="1" min="4" max="4" width="16.38"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,127 +718,128 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="181.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="193.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>